<commit_message>
Updated spreadsheet to have double quotes around entries in Title
</commit_message>
<xml_diff>
--- a/data/Expressions.xlsx
+++ b/data/Expressions.xlsx
@@ -42,9 +42,6 @@
     <t>Current Sales</t>
   </si>
   <si>
-    <t>Cur Ind (' &amp; only(Year) &amp; ')'</t>
-  </si>
-  <si>
     <t>CurrentSales</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>Prior Sales</t>
   </si>
   <si>
-    <t>Pr Sales (' &amp; (only([Year]) - 1) &amp; ')'</t>
-  </si>
-  <si>
     <t>PriorSales</t>
   </si>
   <si>
@@ -72,15 +66,9 @@
     <t>Current Profit</t>
   </si>
   <si>
-    <t>Cur Profit (' &amp; only(Year) &amp; ')'</t>
-  </si>
-  <si>
     <t>Prior Profit</t>
   </si>
   <si>
-    <t>Pr Profit (' &amp; (only(Year) - 1) &amp; ')'</t>
-  </si>
-  <si>
     <t>PriorProfit</t>
   </si>
   <si>
@@ -90,9 +78,6 @@
     <t>Current Margin</t>
   </si>
   <si>
-    <t>Cur Margin (' &amp; only(Year) &amp; ')'</t>
-  </si>
-  <si>
     <t>CurrentMargin</t>
   </si>
   <si>
@@ -102,13 +87,28 @@
     <t>Prior Margin</t>
   </si>
   <si>
-    <t>Pr Margin (' &amp; (only(Year) - 1) &amp; ')'</t>
-  </si>
-  <si>
     <t>PriorMargin</t>
   </si>
   <si>
     <t>$(PriorProfit) / $(PriorSales)</t>
+  </si>
+  <si>
+    <t>"='Cur Ind (' &amp; only(Year) &amp; ')'"</t>
+  </si>
+  <si>
+    <t>"='Pr Sales (' &amp; (only([Year]) - 1) &amp; ')'"</t>
+  </si>
+  <si>
+    <t>"='Pr Profit (' &amp; (only(Year) - 1) &amp; ')'"</t>
+  </si>
+  <si>
+    <t>"='Pr Margin (' &amp; (only(Year) - 1) &amp; ')'"</t>
+  </si>
+  <si>
+    <t>"='Cur Margin (' &amp; only(Year) &amp; ')'"</t>
+  </si>
+  <si>
+    <t>"='Cur Profit (' &amp; only(Year) &amp; ')'"</t>
   </si>
 </sst>
 </file>
@@ -165,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,7 +180,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +483,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -516,14 +515,14 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -531,16 +530,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -548,16 +547,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -565,16 +564,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -582,16 +581,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -599,16 +598,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>

</xml_diff>